<commit_message>
rydder videre i plots -gemini lagde et fancy et
</commit_message>
<xml_diff>
--- a/waveprocessed/PROCESSED-20251113-tett6roof-probeadjusted/meta.xlsx
+++ b/waveprocessed/PROCESSED-20251113-tett6roof-probeadjusted/meta.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DF2"/>
+  <dimension ref="A1:DF13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1059,13 +1059,13 @@
         <v>1.5385</v>
       </c>
       <c r="Y2" t="n">
-        <v>2.048927717267305</v>
+        <v>2.048927717267306</v>
       </c>
       <c r="Z2" t="n">
         <v>3.066572458475788</v>
       </c>
       <c r="AA2" t="n">
-        <v>5.368190619240341</v>
+        <v>5.368190619240342</v>
       </c>
       <c r="AB2" t="n">
         <v>0.0290333057536777</v>
@@ -1112,16 +1112,16 @@
         <v>1.5385</v>
       </c>
       <c r="AR2" t="n">
-        <v>2.048927717267305</v>
+        <v>2.048927717267306</v>
       </c>
       <c r="AS2" t="n">
         <v>3.066572458475788</v>
       </c>
       <c r="AT2" t="n">
-        <v>5.368190619240341</v>
+        <v>5.368190619240342</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.02949431449006288</v>
+        <v>0.02949431449006289</v>
       </c>
       <c r="AV2" t="n">
         <v>0.8300751689623258</v>
@@ -1165,13 +1165,13 @@
         <v>1.5385</v>
       </c>
       <c r="BK2" t="n">
-        <v>2.048927717267305</v>
+        <v>2.048927717267306</v>
       </c>
       <c r="BL2" t="n">
         <v>3.066572458475788</v>
       </c>
       <c r="BM2" t="n">
-        <v>5.368190619240341</v>
+        <v>5.368190619240342</v>
       </c>
       <c r="BN2" t="n">
         <v>0.02905379503085041</v>
@@ -1218,13 +1218,13 @@
         <v>1.5385</v>
       </c>
       <c r="CD2" t="n">
-        <v>2.048927717267305</v>
+        <v>2.048927717267306</v>
       </c>
       <c r="CE2" t="n">
         <v>3.066572458475788</v>
       </c>
       <c r="CF2" t="n">
-        <v>5.368190619240341</v>
+        <v>5.368190619240342</v>
       </c>
       <c r="CG2" t="n">
         <v>0.02898208256074606</v>
@@ -1293,6 +1293,3526 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0300-freq0650-per40-depth580-mstop30-run1.csv</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-11-13T14:04:06</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J3" t="n">
+        <v>40</v>
+      </c>
+      <c r="K3" t="n">
+        <v>580</v>
+      </c>
+      <c r="L3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O3" t="n">
+        <v>268.2338799999999</v>
+      </c>
+      <c r="P3" t="n">
+        <v>3950</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>13180.76923076923</v>
+      </c>
+      <c r="R3" t="n">
+        <v>14.00999999999998</v>
+      </c>
+      <c r="S3" t="n">
+        <v>13.42232842974149</v>
+      </c>
+      <c r="T3" t="n">
+        <v>13.44958715855431</v>
+      </c>
+      <c r="U3" t="n">
+        <v>19.05504887839486</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.3413703667915149</v>
+      </c>
+      <c r="W3" t="n">
+        <v>19.05810645067712</v>
+      </c>
+      <c r="X3" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.02870547731891491</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>269.1222</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>13230.76923076923</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>14.39500000000002</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>14.02577137275203</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>14.07038985315739</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>19.93085419281478</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.267285528602732</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>19.93264634736299</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.02949431449006292</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>269.92904</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>14.345</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>13.52075362159465</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>13.55093954431222</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>19.18533476185031</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.363245162365084</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>19.18877320133425</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>0.0293918681041995</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="BQ3" t="inlineStr"/>
+      <c r="BR3" t="inlineStr"/>
+      <c r="BS3" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>270.3004</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>14.205</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>13.53672403823337</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>13.56220250631503</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>19.21006400448165</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>0.3458847940395066</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>19.21317764834931</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="CF3" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>0.02910501822378208</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="CJ3" t="inlineStr"/>
+      <c r="CK3" t="inlineStr"/>
+      <c r="CL3" t="inlineStr"/>
+      <c r="CM3" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO3" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP3" t="n">
+        <v>0.029495334920285</v>
+      </c>
+      <c r="CQ3" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR3" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS3" t="n">
+        <v>1.993203138117973</v>
+      </c>
+      <c r="CT3" t="inlineStr"/>
+      <c r="CU3" t="inlineStr"/>
+      <c r="CV3" t="inlineStr"/>
+      <c r="CW3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX3" t="inlineStr"/>
+      <c r="CY3" t="n">
+        <v>1.044958141664409</v>
+      </c>
+      <c r="CZ3" t="n">
+        <v>0.9639935845426311</v>
+      </c>
+      <c r="DA3" t="n">
+        <v>1.001181177993896</v>
+      </c>
+      <c r="DB3" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DC3" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DD3" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DE3" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DF3" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0100-freq1300-per40-depth580-mstop30-run2freqedit.csv</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-11-13T14:22:16</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K4" t="n">
+        <v>580</v>
+      </c>
+      <c r="L4" t="n">
+        <v>30</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O4" t="n">
+        <v>268.24456</v>
+      </c>
+      <c r="P4" t="n">
+        <v>4700</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>9315.384615384615</v>
+      </c>
+      <c r="R4" t="n">
+        <v>8.204999999999984</v>
+      </c>
+      <c r="S4" t="n">
+        <v>7.765994905564461</v>
+      </c>
+      <c r="T4" t="n">
+        <v>7.757917169784386</v>
+      </c>
+      <c r="U4" t="n">
+        <v>10.99382980878394</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.8049946182497736</v>
+      </c>
+      <c r="W4" t="n">
+        <v>11.02326223038886</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.0558485567176684</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>269.21236</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>4800</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>9415.384615384615</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>8.590000000000003</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>7.579529908133033</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>7.553696594468446</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>10.70701874225898</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.7988329365695356</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>10.73677718906532</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.05846911666115451</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>269.94156</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>4.685000000000002</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>4.225205845148875</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>4.262918058704027</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>6.03651586897569</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>0.5061445081428362</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>6.057698085867146</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>0.03188915152008252</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
+      <c r="BS4" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>270.3052</v>
+      </c>
+      <c r="BU4" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>4.97999999999999</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>4.60986156107696</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>4.618496801254325</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>6.542678820053996</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>0.5154208947229395</v>
+      </c>
+      <c r="CB4" t="n">
+        <v>6.562949401077243</v>
+      </c>
+      <c r="CC4" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="CE4" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="CF4" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="CG4" t="n">
+        <v>0.03389711303522103</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="CJ4" t="inlineStr"/>
+      <c r="CK4" t="inlineStr"/>
+      <c r="CL4" t="inlineStr"/>
+      <c r="CM4" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN4" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO4" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP4" t="n">
+        <v>0.05848461839031356</v>
+      </c>
+      <c r="CQ4" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR4" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS4" t="n">
+        <v>1.19970570478913</v>
+      </c>
+      <c r="CT4" t="inlineStr"/>
+      <c r="CU4" t="inlineStr"/>
+      <c r="CV4" t="inlineStr"/>
+      <c r="CW4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX4" t="inlineStr"/>
+      <c r="CY4" t="n">
+        <v>0.9759895545002453</v>
+      </c>
+      <c r="CZ4" t="n">
+        <v>0.5574495907213348</v>
+      </c>
+      <c r="DA4" t="n">
+        <v>1.091038337545074</v>
+      </c>
+      <c r="DB4" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DC4" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DD4" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DE4" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DF4" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0200-freq1300-per40-depth580-mstop30-run2.csv</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-11-13T14:27:58</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K5" t="n">
+        <v>580</v>
+      </c>
+      <c r="L5" t="n">
+        <v>30</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O5" t="n">
+        <v>268.24488</v>
+      </c>
+      <c r="P5" t="n">
+        <v>4700</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>9315.384615384615</v>
+      </c>
+      <c r="R5" t="n">
+        <v>16.45000000000002</v>
+      </c>
+      <c r="S5" t="n">
+        <v>15.3820833441514</v>
+      </c>
+      <c r="T5" t="n">
+        <v>15.43274601674943</v>
+      </c>
+      <c r="U5" t="n">
+        <v>21.85503350622304</v>
+      </c>
+      <c r="V5" t="n">
+        <v>1.443089770715056</v>
+      </c>
+      <c r="W5" t="n">
+        <v>21.90262535963381</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.1119693794034915</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>269.1368400000001</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>4800</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>9415.384615384615</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>17.175</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>15.57744222729847</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>15.58955383027241</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>22.08755203083409</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>1.691709426532427</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>22.152242222823</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.1169042000762896</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AX5" t="inlineStr"/>
+      <c r="AY5" t="inlineStr"/>
+      <c r="AZ5" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>269.93292</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>11.59962500000002</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>10.43768077345858</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>10.28161121575724</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>14.56158433982026</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>0.9403061375227209</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>14.59191262713568</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>0.07895457827132076</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="BQ5" t="inlineStr"/>
+      <c r="BR5" t="inlineStr"/>
+      <c r="BS5" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT5" t="n">
+        <v>270.30552</v>
+      </c>
+      <c r="BU5" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BV5" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BW5" t="n">
+        <v>11.94</v>
+      </c>
+      <c r="BX5" t="n">
+        <v>10.71886619761013</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>10.51988588277293</v>
+      </c>
+      <c r="BZ5" t="n">
+        <v>14.89877312710286</v>
+      </c>
+      <c r="CA5" t="n">
+        <v>0.9209874021612224</v>
+      </c>
+      <c r="CB5" t="n">
+        <v>14.92721201322679</v>
+      </c>
+      <c r="CC5" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="CD5" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="CE5" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="CF5" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="CG5" t="n">
+        <v>0.08127139149408433</v>
+      </c>
+      <c r="CH5" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="CI5" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="CJ5" t="inlineStr"/>
+      <c r="CK5" t="inlineStr"/>
+      <c r="CL5" t="inlineStr"/>
+      <c r="CM5" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN5" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO5" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP5" t="n">
+        <v>0.1169351945114825</v>
+      </c>
+      <c r="CQ5" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR5" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS5" t="n">
+        <v>1.19970570478913</v>
+      </c>
+      <c r="CT5" t="inlineStr"/>
+      <c r="CU5" t="inlineStr"/>
+      <c r="CV5" t="inlineStr"/>
+      <c r="CW5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX5" t="inlineStr"/>
+      <c r="CY5" t="n">
+        <v>1.012700417672704</v>
+      </c>
+      <c r="CZ5" t="n">
+        <v>0.6700510020295386</v>
+      </c>
+      <c r="DA5" t="n">
+        <v>1.026939454295878</v>
+      </c>
+      <c r="DB5" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DC5" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DD5" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DE5" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DF5" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0100-freq0650-per40-depth580-mstop30-run1.csv</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-11-13T14:18:10</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J6" t="n">
+        <v>40</v>
+      </c>
+      <c r="K6" t="n">
+        <v>580</v>
+      </c>
+      <c r="L6" t="n">
+        <v>30</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O6" t="n">
+        <v>268.24424</v>
+      </c>
+      <c r="P6" t="n">
+        <v>3950</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>13180.76923076923</v>
+      </c>
+      <c r="R6" t="n">
+        <v>4.765000000000043</v>
+      </c>
+      <c r="S6" t="n">
+        <v>4.466587939463903</v>
+      </c>
+      <c r="T6" t="n">
+        <v>4.47286682006346</v>
+      </c>
+      <c r="U6" t="n">
+        <v>6.332877283356077</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.1482185811424163</v>
+      </c>
+      <c r="W6" t="n">
+        <v>6.334611545615353</v>
+      </c>
+      <c r="X6" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.009763140572778802</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>269.15068</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>13230.76923076923</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>4.990000000000009</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>4.761394595115003</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>4.777669612632569</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>6.7642375398165</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.2887598875440304</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>6.770398198608205</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.01022414930916388</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AX6" t="inlineStr"/>
+      <c r="AY6" t="inlineStr"/>
+      <c r="AZ6" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>269.92256</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>4.685000000000002</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>4.537184411863327</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>4.546785977084594</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>6.436822847883769</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>0.124279134216022</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>6.438022497494087</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="BN6" t="n">
+        <v>0.009599226355397334</v>
+      </c>
+      <c r="BO6" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="BP6" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="BQ6" t="inlineStr"/>
+      <c r="BR6" t="inlineStr"/>
+      <c r="BS6" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT6" t="n">
+        <v>270.30996</v>
+      </c>
+      <c r="BU6" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BV6" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BW6" t="n">
+        <v>4.900000000000006</v>
+      </c>
+      <c r="BX6" t="n">
+        <v>4.553831742377166</v>
+      </c>
+      <c r="BY6" t="n">
+        <v>4.566138959534992</v>
+      </c>
+      <c r="BZ6" t="n">
+        <v>6.462775153819909</v>
+      </c>
+      <c r="CA6" t="n">
+        <v>0.1219614582796841</v>
+      </c>
+      <c r="CB6" t="n">
+        <v>6.463925841633524</v>
+      </c>
+      <c r="CC6" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="CD6" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="CE6" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="CF6" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="CG6" t="n">
+        <v>0.01003974581460981</v>
+      </c>
+      <c r="CH6" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="CI6" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="CJ6" t="inlineStr"/>
+      <c r="CK6" t="inlineStr"/>
+      <c r="CL6" t="inlineStr"/>
+      <c r="CM6" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN6" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO6" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP6" t="n">
+        <v>0.01022450303940411</v>
+      </c>
+      <c r="CQ6" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR6" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS6" t="n">
+        <v>1.993203138117973</v>
+      </c>
+      <c r="CT6" t="inlineStr"/>
+      <c r="CU6" t="inlineStr"/>
+      <c r="CV6" t="inlineStr"/>
+      <c r="CW6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX6" t="inlineStr"/>
+      <c r="CY6" t="n">
+        <v>1.066002653400458</v>
+      </c>
+      <c r="CZ6" t="n">
+        <v>0.9529108166162691</v>
+      </c>
+      <c r="DA6" t="n">
+        <v>1.003669088360242</v>
+      </c>
+      <c r="DB6" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DC6" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DD6" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DE6" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DF6" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0200-freq1300-per40-depth580-mstop30-run1.csv</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-11-13T13:55:38</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J7" t="n">
+        <v>40</v>
+      </c>
+      <c r="K7" t="n">
+        <v>580</v>
+      </c>
+      <c r="L7" t="n">
+        <v>30</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O7" t="n">
+        <v>268.18424</v>
+      </c>
+      <c r="P7" t="n">
+        <v>4700</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>9315.384615384615</v>
+      </c>
+      <c r="R7" t="n">
+        <v>16.571625</v>
+      </c>
+      <c r="S7" t="n">
+        <v>15.36368127965209</v>
+      </c>
+      <c r="T7" t="n">
+        <v>15.32471651337812</v>
+      </c>
+      <c r="U7" t="n">
+        <v>21.71513050950301</v>
+      </c>
+      <c r="V7" t="n">
+        <v>1.361468246080665</v>
+      </c>
+      <c r="W7" t="n">
+        <v>21.75776847082059</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.1127972381129108</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>269.22428</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>4800</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>9415.384615384615</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>16.91999999999999</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>15.13900888794337</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>15.11215001418798</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>21.4199812528712</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>1.444652678474364</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>21.46864267332187</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.1151685045293054</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AX7" t="inlineStr"/>
+      <c r="AY7" t="inlineStr"/>
+      <c r="AZ7" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>269.87508</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>11.58699999999999</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>10.47550187605715</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>10.26958488270075</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>14.55348179334477</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>0.9856673324442503</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>14.58682187453681</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>0.07886864432512179</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="BQ7" t="inlineStr"/>
+      <c r="BR7" t="inlineStr"/>
+      <c r="BS7" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT7" t="n">
+        <v>270.25808</v>
+      </c>
+      <c r="BU7" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BV7" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BW7" t="n">
+        <v>12.15000000000001</v>
+      </c>
+      <c r="BX7" t="n">
+        <v>10.98971671903447</v>
+      </c>
+      <c r="BY7" t="n">
+        <v>10.71107957188797</v>
+      </c>
+      <c r="BZ7" t="n">
+        <v>15.17580518877463</v>
+      </c>
+      <c r="CA7" t="n">
+        <v>1.117769082247855</v>
+      </c>
+      <c r="CB7" t="n">
+        <v>15.21691397257894</v>
+      </c>
+      <c r="CC7" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="CD7" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="CE7" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="CF7" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="CG7" t="n">
+        <v>0.08270078782689491</v>
+      </c>
+      <c r="CH7" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="CI7" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="CJ7" t="inlineStr"/>
+      <c r="CK7" t="inlineStr"/>
+      <c r="CL7" t="inlineStr"/>
+      <c r="CM7" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN7" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO7" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP7" t="n">
+        <v>0.1151990387851111</v>
+      </c>
+      <c r="CQ7" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR7" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS7" t="n">
+        <v>1.19970570478913</v>
+      </c>
+      <c r="CT7" t="inlineStr"/>
+      <c r="CU7" t="inlineStr"/>
+      <c r="CV7" t="inlineStr"/>
+      <c r="CW7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX7" t="inlineStr"/>
+      <c r="CY7" t="n">
+        <v>0.9853763959549013</v>
+      </c>
+      <c r="CZ7" t="n">
+        <v>0.6919542721452389</v>
+      </c>
+      <c r="DA7" t="n">
+        <v>1.049087370615876</v>
+      </c>
+      <c r="DB7" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DC7" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DD7" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DE7" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DF7" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0100-freq0650-per40-depth580-mstop30-run2.csv</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-11-13T14:43:50</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J8" t="n">
+        <v>40</v>
+      </c>
+      <c r="K8" t="n">
+        <v>580</v>
+      </c>
+      <c r="L8" t="n">
+        <v>30</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O8" t="n">
+        <v>268.23384</v>
+      </c>
+      <c r="P8" t="n">
+        <v>3950</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>13180.76923076923</v>
+      </c>
+      <c r="R8" t="n">
+        <v>4.760000000000019</v>
+      </c>
+      <c r="S8" t="n">
+        <v>4.463426674776379</v>
+      </c>
+      <c r="T8" t="n">
+        <v>4.467438373159494</v>
+      </c>
+      <c r="U8" t="n">
+        <v>6.32660677547944</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.1381512955042459</v>
+      </c>
+      <c r="W8" t="n">
+        <v>6.328114969877827</v>
+      </c>
+      <c r="X8" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.009752895934192415</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>269.1144399999999</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>13230.76923076923</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>4.939999999999998</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>4.745273257178552</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>4.756960419424226</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>6.737386818225323</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>0.2956969747639679</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>6.743872614401972</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0.01012170292330049</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AX8" t="inlineStr"/>
+      <c r="AY8" t="inlineStr"/>
+      <c r="AZ8" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>269.91976</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>4.685000000000002</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>4.532408429431563</v>
+      </c>
+      <c r="BF8" t="n">
+        <v>4.53805266710841</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>6.424909678986146</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>0.1176926988532854</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>6.425987547022887</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="BN8" t="n">
+        <v>0.009599226355397334</v>
+      </c>
+      <c r="BO8" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="BP8" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="BQ8" t="inlineStr"/>
+      <c r="BR8" t="inlineStr"/>
+      <c r="BS8" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT8" t="n">
+        <v>270.29384</v>
+      </c>
+      <c r="BU8" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BV8" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BW8" t="n">
+        <v>4.764999999999986</v>
+      </c>
+      <c r="BX8" t="n">
+        <v>4.554450153243205</v>
+      </c>
+      <c r="BY8" t="n">
+        <v>4.565419149842276</v>
+      </c>
+      <c r="BZ8" t="n">
+        <v>6.461086463077217</v>
+      </c>
+      <c r="CA8" t="n">
+        <v>0.1193276153179478</v>
+      </c>
+      <c r="CB8" t="n">
+        <v>6.462188279765388</v>
+      </c>
+      <c r="CC8" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="CD8" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="CE8" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="CF8" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="CG8" t="n">
+        <v>0.009763140572778684</v>
+      </c>
+      <c r="CH8" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="CI8" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="CJ8" t="inlineStr"/>
+      <c r="CK8" t="inlineStr"/>
+      <c r="CL8" t="inlineStr"/>
+      <c r="CM8" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN8" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO8" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP8" t="n">
+        <v>0.01012205310914954</v>
+      </c>
+      <c r="CQ8" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR8" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS8" t="n">
+        <v>1.993203138117973</v>
+      </c>
+      <c r="CT8" t="inlineStr"/>
+      <c r="CU8" t="inlineStr"/>
+      <c r="CV8" t="inlineStr"/>
+      <c r="CW8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX8" t="inlineStr"/>
+      <c r="CY8" t="n">
+        <v>1.063145785276353</v>
+      </c>
+      <c r="CZ8" t="n">
+        <v>0.9551417134039705</v>
+      </c>
+      <c r="DA8" t="n">
+        <v>1.00486313714989</v>
+      </c>
+      <c r="DB8" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DC8" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DD8" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DE8" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DF8" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0200-freq0650-per40-depth580-mstop30-run2.csv</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-11-13T14:41:34</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J9" t="n">
+        <v>40</v>
+      </c>
+      <c r="K9" t="n">
+        <v>580</v>
+      </c>
+      <c r="L9" t="n">
+        <v>30</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O9" t="n">
+        <v>268.2058000000001</v>
+      </c>
+      <c r="P9" t="n">
+        <v>3950</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>13180.76923076923</v>
+      </c>
+      <c r="R9" t="n">
+        <v>14.16999999999999</v>
+      </c>
+      <c r="S9" t="n">
+        <v>13.49754757669499</v>
+      </c>
+      <c r="T9" t="n">
+        <v>13.52044672719136</v>
+      </c>
+      <c r="U9" t="n">
+        <v>19.14596832148539</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.3286542233728085</v>
+      </c>
+      <c r="W9" t="n">
+        <v>19.14878890598209</v>
+      </c>
+      <c r="X9" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.0290333057536777</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>269.3912800000001</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>13230.76923076923</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>14.39500000000001</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>13.92684205585111</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>13.96087546148221</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>19.76720473943299</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>0.3101831145493709</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>19.76963825605348</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.02949431449006289</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AX9" t="inlineStr"/>
+      <c r="AY9" t="inlineStr"/>
+      <c r="AZ9" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>269.8854400000001</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>14.18000000000001</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>13.46149289537729</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>13.48659953383576</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>19.09648203498408</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>0.3698213823148598</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>19.10006266919789</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="BN9" t="n">
+        <v>0.02905379503085041</v>
+      </c>
+      <c r="BO9" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="BP9" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="BQ9" t="inlineStr"/>
+      <c r="BR9" t="inlineStr"/>
+      <c r="BS9" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT9" t="n">
+        <v>270.2714</v>
+      </c>
+      <c r="BU9" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BV9" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BW9" t="n">
+        <v>14.14500000000001</v>
+      </c>
+      <c r="BX9" t="n">
+        <v>13.50250950419938</v>
+      </c>
+      <c r="BY9" t="n">
+        <v>13.52145995282447</v>
+      </c>
+      <c r="BZ9" t="n">
+        <v>19.15160510737817</v>
+      </c>
+      <c r="CA9" t="n">
+        <v>0.2860490150336762</v>
+      </c>
+      <c r="CB9" t="n">
+        <v>19.15374120708421</v>
+      </c>
+      <c r="CC9" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="CD9" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="CE9" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="CF9" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="CG9" t="n">
+        <v>0.02898208256074606</v>
+      </c>
+      <c r="CH9" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="CI9" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="CJ9" t="inlineStr"/>
+      <c r="CK9" t="inlineStr"/>
+      <c r="CL9" t="inlineStr"/>
+      <c r="CM9" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN9" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO9" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP9" t="n">
+        <v>0.02949533492028497</v>
+      </c>
+      <c r="CQ9" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR9" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS9" t="n">
+        <v>1.993203138117973</v>
+      </c>
+      <c r="CT9" t="inlineStr"/>
+      <c r="CU9" t="inlineStr"/>
+      <c r="CV9" t="inlineStr"/>
+      <c r="CW9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX9" t="inlineStr"/>
+      <c r="CY9" t="n">
+        <v>1.031805368843252</v>
+      </c>
+      <c r="CZ9" t="n">
+        <v>0.966586168019453</v>
+      </c>
+      <c r="DA9" t="n">
+        <v>1.003046958397621</v>
+      </c>
+      <c r="DB9" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DC9" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DD9" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DE9" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DF9" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0100-freq1300-per40-depth580-mstop30-run1.csv</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-11-13T13:53:36</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J10" t="n">
+        <v>40</v>
+      </c>
+      <c r="K10" t="n">
+        <v>580</v>
+      </c>
+      <c r="L10" t="n">
+        <v>30</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O10" t="n">
+        <v>267.9305199999999</v>
+      </c>
+      <c r="P10" t="n">
+        <v>4700</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>9315.384615384615</v>
+      </c>
+      <c r="R10" t="n">
+        <v>8.204624999999984</v>
+      </c>
+      <c r="S10" t="n">
+        <v>7.610735445519395</v>
+      </c>
+      <c r="T10" t="n">
+        <v>7.521227679893078</v>
+      </c>
+      <c r="U10" t="n">
+        <v>10.6602714490858</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.843694038361686</v>
+      </c>
+      <c r="W10" t="n">
+        <v>10.69360589317564</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.05584600422421696</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>269.11424</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>4800</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>9415.384615384615</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>8.585000000000008</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>7.639430814155629</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>7.680480419435562</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>10.88927137797308</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>1.188496185280038</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>10.95393784561374</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0.05843508341513523</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AX10" t="inlineStr"/>
+      <c r="AY10" t="inlineStr"/>
+      <c r="AZ10" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>269.84968</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>4.891625000000017</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>4.375138630156265</v>
+      </c>
+      <c r="BF10" t="n">
+        <v>4.356333896248159</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>6.168891490702194</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>0.4204284769934745</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>6.18320162442767</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="BN10" t="n">
+        <v>0.03329557541183013</v>
+      </c>
+      <c r="BO10" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="BP10" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="BQ10" t="inlineStr"/>
+      <c r="BR10" t="inlineStr"/>
+      <c r="BS10" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT10" t="n">
+        <v>270.24552</v>
+      </c>
+      <c r="BU10" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BV10" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BW10" t="n">
+        <v>5.109999999999957</v>
+      </c>
+      <c r="BX10" t="n">
+        <v>4.655646048983599</v>
+      </c>
+      <c r="BY10" t="n">
+        <v>4.623659802630424</v>
+      </c>
+      <c r="BZ10" t="n">
+        <v>6.546975857413639</v>
+      </c>
+      <c r="CA10" t="n">
+        <v>0.3536660965835061</v>
+      </c>
+      <c r="CB10" t="n">
+        <v>6.556521378401024</v>
+      </c>
+      <c r="CC10" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="CD10" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="CE10" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="CF10" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="CG10" t="n">
+        <v>0.03478197743172257</v>
+      </c>
+      <c r="CH10" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="CI10" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="CJ10" t="inlineStr"/>
+      <c r="CK10" t="inlineStr"/>
+      <c r="CL10" t="inlineStr"/>
+      <c r="CM10" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN10" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO10" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP10" t="n">
+        <v>0.05845057612116905</v>
+      </c>
+      <c r="CQ10" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR10" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS10" t="n">
+        <v>1.19970570478913</v>
+      </c>
+      <c r="CT10" t="inlineStr"/>
+      <c r="CU10" t="inlineStr"/>
+      <c r="CV10" t="inlineStr"/>
+      <c r="CW10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX10" t="inlineStr"/>
+      <c r="CY10" t="n">
+        <v>1.003770380516002</v>
+      </c>
+      <c r="CZ10" t="n">
+        <v>0.5727047913110579</v>
+      </c>
+      <c r="DA10" t="n">
+        <v>1.064113949874387</v>
+      </c>
+      <c r="DB10" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DC10" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DD10" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DE10" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DF10" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0200-freq0650-per40-depth580-mstop30-run1.csv</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-11-13T14:09:22</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J11" t="n">
+        <v>40</v>
+      </c>
+      <c r="K11" t="n">
+        <v>580</v>
+      </c>
+      <c r="L11" t="n">
+        <v>30</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O11" t="n">
+        <v>268.24364</v>
+      </c>
+      <c r="P11" t="n">
+        <v>3950</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>13180.76923076923</v>
+      </c>
+      <c r="R11" t="n">
+        <v>9.449999999999989</v>
+      </c>
+      <c r="S11" t="n">
+        <v>8.909724015460217</v>
+      </c>
+      <c r="T11" t="n">
+        <v>8.926956589859223</v>
+      </c>
+      <c r="U11" t="n">
+        <v>12.64597595453074</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.2603378387749886</v>
+      </c>
+      <c r="W11" t="n">
+        <v>12.6486554081004</v>
+      </c>
+      <c r="X11" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.01936236692817602</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>269.26376</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>13230.76923076923</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>9.651250000000001</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>9.313881644165752</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>9.338443257302391</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>13.22347201279226</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>0.3013558859152358</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>13.22690543714122</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.01977471363127609</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="AX11" t="inlineStr"/>
+      <c r="AY11" t="inlineStr"/>
+      <c r="AZ11" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>269.93192</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>9.490000000000009</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>8.988954477913905</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>9.007302457046562</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>12.75082312577516</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>0.2732757948259791</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>12.75375121463643</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="BN11" t="n">
+        <v>0.01944432403686675</v>
+      </c>
+      <c r="BO11" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="BP11" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="BQ11" t="inlineStr"/>
+      <c r="BR11" t="inlineStr"/>
+      <c r="BS11" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT11" t="n">
+        <v>270.33268</v>
+      </c>
+      <c r="BU11" t="n">
+        <v>4500</v>
+      </c>
+      <c r="BV11" t="n">
+        <v>13730.76923076923</v>
+      </c>
+      <c r="BW11" t="n">
+        <v>9.520500000000006</v>
+      </c>
+      <c r="BX11" t="n">
+        <v>9.040913352788527</v>
+      </c>
+      <c r="BY11" t="n">
+        <v>9.058105245000101</v>
+      </c>
+      <c r="BZ11" t="n">
+        <v>12.82644039419034</v>
+      </c>
+      <c r="CA11" t="n">
+        <v>0.2567353775844811</v>
+      </c>
+      <c r="CB11" t="n">
+        <v>12.82900955802205</v>
+      </c>
+      <c r="CC11" t="n">
+        <v>1.5385</v>
+      </c>
+      <c r="CD11" t="n">
+        <v>2.048927717267306</v>
+      </c>
+      <c r="CE11" t="n">
+        <v>3.066572458475788</v>
+      </c>
+      <c r="CF11" t="n">
+        <v>5.368190619240342</v>
+      </c>
+      <c r="CG11" t="n">
+        <v>0.0195068163322434</v>
+      </c>
+      <c r="CH11" t="n">
+        <v>0.8300751689623258</v>
+      </c>
+      <c r="CI11" t="n">
+        <v>1.993222267452576</v>
+      </c>
+      <c r="CJ11" t="inlineStr"/>
+      <c r="CK11" t="inlineStr"/>
+      <c r="CL11" t="inlineStr"/>
+      <c r="CM11" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN11" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO11" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP11" t="n">
+        <v>0.01977539778738452</v>
+      </c>
+      <c r="CQ11" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR11" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS11" t="n">
+        <v>1.993203138117973</v>
+      </c>
+      <c r="CT11" t="inlineStr"/>
+      <c r="CU11" t="inlineStr"/>
+      <c r="CV11" t="inlineStr"/>
+      <c r="CW11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX11" t="inlineStr"/>
+      <c r="CY11" t="n">
+        <v>1.045361408277545</v>
+      </c>
+      <c r="CZ11" t="n">
+        <v>0.9651136681068541</v>
+      </c>
+      <c r="DA11" t="n">
+        <v>1.005780302370235</v>
+      </c>
+      <c r="DB11" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DC11" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DD11" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DE11" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DF11" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0300-freq1300-per40-depth580-mstop30-run2.csv</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-11-13T14:30:24</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J12" t="n">
+        <v>40</v>
+      </c>
+      <c r="K12" t="n">
+        <v>580</v>
+      </c>
+      <c r="L12" t="n">
+        <v>30</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O12" t="n">
+        <v>268.1942</v>
+      </c>
+      <c r="P12" t="n">
+        <v>4700</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>9315.384615384615</v>
+      </c>
+      <c r="R12" t="n">
+        <v>26.44350000000001</v>
+      </c>
+      <c r="S12" t="n">
+        <v>22.43734566759758</v>
+      </c>
+      <c r="T12" t="n">
+        <v>22.29375605983603</v>
+      </c>
+      <c r="U12" t="n">
+        <v>31.72527711409117</v>
+      </c>
+      <c r="V12" t="n">
+        <v>5.138302767115129</v>
+      </c>
+      <c r="W12" t="n">
+        <v>32.1386895080123</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.179991628222263</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>269.17764</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>4800</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>9415.384615384615</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>24.43662499999999</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>22.76109082278461</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>22.97789251033586</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>32.54346240527122</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>2.242103322302194</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>32.62060656442765</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0.7693333333333332</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>6.80664920385966</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>0.9230952145464986</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>17.83342091411231</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.166331534101267</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.9992556045629514</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>1.199863797070839</v>
+      </c>
+      <c r="AX12" t="inlineStr"/>
+      <c r="AY12" t="inlineStr"/>
+      <c r="AZ12" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>269.62976</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>17.81965000000001</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>16.38217326895289</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>16.35943301093564</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>23.18546295718482</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>1.901337404939653</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>23.2632924683161</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>0.7691666666666667</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>6.809582094531432</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>0.9226976369409542</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>17.84110508767235</v>
+      </c>
+      <c r="BN12" t="n">
+        <v>0.1213443695708171</v>
+      </c>
+      <c r="BO12" t="n">
+        <v>0.9992581318692667</v>
+      </c>
+      <c r="BP12" t="n">
+        <v>1.199606895264513</v>
+      </c>
+      <c r="BQ12" t="inlineStr"/>
+      <c r="BR12" t="inlineStr"/>
+      <c r="BS12" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT12" t="n">
+        <v>270.30488</v>
+      </c>
+      <c r="BU12" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BV12" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BW12" t="n">
+        <v>22.59990000000013</v>
+      </c>
+      <c r="BX12" t="n">
+        <v>16.73732343624379</v>
+      </c>
+      <c r="BY12" t="n">
+        <v>17.01478280939623</v>
+      </c>
+      <c r="BZ12" t="n">
+        <v>24.40045445801821</v>
+      </c>
+      <c r="CA12" t="n">
+        <v>6.815740633325402</v>
+      </c>
+      <c r="CB12" t="n">
+        <v>25.33449226131409</v>
+      </c>
+      <c r="CC12" t="n">
+        <v>0.7691666666666667</v>
+      </c>
+      <c r="CD12" t="n">
+        <v>6.809582094531432</v>
+      </c>
+      <c r="CE12" t="n">
+        <v>0.9226976369409542</v>
+      </c>
+      <c r="CF12" t="n">
+        <v>17.84110508767235</v>
+      </c>
+      <c r="CG12" t="n">
+        <v>0.1538958743782018</v>
+      </c>
+      <c r="CH12" t="n">
+        <v>0.9992581318692667</v>
+      </c>
+      <c r="CI12" t="n">
+        <v>1.199606895264513</v>
+      </c>
+      <c r="CJ12" t="inlineStr"/>
+      <c r="CK12" t="inlineStr"/>
+      <c r="CL12" t="inlineStr"/>
+      <c r="CM12" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN12" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO12" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP12" t="n">
+        <v>0.1663756330468213</v>
+      </c>
+      <c r="CQ12" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR12" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS12" t="n">
+        <v>1.19970570478913</v>
+      </c>
+      <c r="CT12" t="inlineStr"/>
+      <c r="CU12" t="inlineStr"/>
+      <c r="CV12" t="inlineStr"/>
+      <c r="CW12" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX12" t="inlineStr"/>
+      <c r="CY12" t="n">
+        <v>1.014428852680848</v>
+      </c>
+      <c r="CZ12" t="n">
+        <v>0.7197446465330996</v>
+      </c>
+      <c r="DA12" t="n">
+        <v>1.021679063055936</v>
+      </c>
+      <c r="DB12" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DC12" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DD12" t="n">
+        <v>1.300108342361864</v>
+      </c>
+      <c r="DE12" t="n">
+        <v>1.300108342361864</v>
+      </c>
+      <c r="DF12" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251113-tett6roof-probeadjusted/reversepanel-nowind-amp0300-freq1300-per40-depth580-mstop30-run1.csv</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-11-13T13:58:24</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>reverse</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J13" t="n">
+        <v>40</v>
+      </c>
+      <c r="K13" t="n">
+        <v>580</v>
+      </c>
+      <c r="L13" t="n">
+        <v>30</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O13" t="n">
+        <v>268.1828</v>
+      </c>
+      <c r="P13" t="n">
+        <v>4700</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>9315.384615384615</v>
+      </c>
+      <c r="R13" t="n">
+        <v>25.66589999999999</v>
+      </c>
+      <c r="S13" t="n">
+        <v>22.38152814576669</v>
+      </c>
+      <c r="T13" t="n">
+        <v>22.42783791685394</v>
+      </c>
+      <c r="U13" t="n">
+        <v>31.77180482704005</v>
+      </c>
+      <c r="V13" t="n">
+        <v>2.621626983935902</v>
+      </c>
+      <c r="W13" t="n">
+        <v>31.87978215123852</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.7691666666666667</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>6.809582094531432</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.9226976369409542</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>17.84110508767235</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.1747740530800342</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.9992581318692667</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>1.199606895264513</v>
+      </c>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="n">
+        <v>9455</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>269.17108</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>4800</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>9415.384615384615</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>24.73</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>22.94501973248738</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>23.07928052004403</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>32.70009215438801</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>2.030081435247185</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>32.76304713452648</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0.7691666666666667</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>6.809582094531432</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0.9226976369409542</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>17.84110508767235</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>0.1684009651977623</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>0.9992581318692667</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>1.199606895264513</v>
+      </c>
+      <c r="AX13" t="inlineStr"/>
+      <c r="AY13" t="inlineStr"/>
+      <c r="AZ13" t="n">
+        <v>12544</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>269.874</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>17.25965</v>
+      </c>
+      <c r="BE13" t="n">
+        <v>15.55545317250909</v>
+      </c>
+      <c r="BF13" t="n">
+        <v>15.44606469353615</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>21.89297589242492</v>
+      </c>
+      <c r="BH13" t="n">
+        <v>1.968983919546509</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>21.98133961117319</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>0.7691666666666667</v>
+      </c>
+      <c r="BK13" t="n">
+        <v>6.809582094531432</v>
+      </c>
+      <c r="BL13" t="n">
+        <v>0.9226976369409542</v>
+      </c>
+      <c r="BM13" t="n">
+        <v>17.84110508767235</v>
+      </c>
+      <c r="BN13" t="n">
+        <v>0.1175310035978795</v>
+      </c>
+      <c r="BO13" t="n">
+        <v>0.9992581318692667</v>
+      </c>
+      <c r="BP13" t="n">
+        <v>1.199606895264513</v>
+      </c>
+      <c r="BQ13" t="inlineStr"/>
+      <c r="BR13" t="inlineStr"/>
+      <c r="BS13" t="n">
+        <v>12545</v>
+      </c>
+      <c r="BT13" t="n">
+        <v>270.24584</v>
+      </c>
+      <c r="BU13" t="n">
+        <v>6500</v>
+      </c>
+      <c r="BV13" t="n">
+        <v>11115.38461538462</v>
+      </c>
+      <c r="BW13" t="n">
+        <v>17.60185000000003</v>
+      </c>
+      <c r="BX13" t="n">
+        <v>15.84656837678451</v>
+      </c>
+      <c r="BY13" t="n">
+        <v>15.64168540736399</v>
+      </c>
+      <c r="BZ13" t="n">
+        <v>22.1986376521759</v>
+      </c>
+      <c r="CA13" t="n">
+        <v>3.781895093747857</v>
+      </c>
+      <c r="CB13" t="n">
+        <v>22.51848671897638</v>
+      </c>
+      <c r="CC13" t="n">
+        <v>0.7691666666666667</v>
+      </c>
+      <c r="CD13" t="n">
+        <v>6.809582094531432</v>
+      </c>
+      <c r="CE13" t="n">
+        <v>0.9226976369409542</v>
+      </c>
+      <c r="CF13" t="n">
+        <v>17.84110508767235</v>
+      </c>
+      <c r="CG13" t="n">
+        <v>0.1198612425906283</v>
+      </c>
+      <c r="CH13" t="n">
+        <v>0.9992581318692667</v>
+      </c>
+      <c r="CI13" t="n">
+        <v>1.199606895264513</v>
+      </c>
+      <c r="CJ13" t="inlineStr"/>
+      <c r="CK13" t="inlineStr"/>
+      <c r="CL13" t="inlineStr"/>
+      <c r="CM13" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN13" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO13" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP13" t="n">
+        <v>0.1683730631888771</v>
+      </c>
+      <c r="CQ13" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR13" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS13" t="n">
+        <v>1.19970570478913</v>
+      </c>
+      <c r="CT13" t="inlineStr"/>
+      <c r="CU13" t="inlineStr"/>
+      <c r="CV13" t="inlineStr"/>
+      <c r="CW13" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX13" t="inlineStr"/>
+      <c r="CY13" t="n">
+        <v>1.025176635976363</v>
+      </c>
+      <c r="CZ13" t="n">
+        <v>0.6779446413151015</v>
+      </c>
+      <c r="DA13" t="n">
+        <v>1.018714672021893</v>
+      </c>
+      <c r="DB13" t="n">
+        <v>1.300108342361864</v>
+      </c>
+      <c r="DC13" t="n">
+        <v>1.300108342361864</v>
+      </c>
+      <c r="DD13" t="n">
+        <v>1.300108342361864</v>
+      </c>
+      <c r="DE13" t="n">
+        <v>1.300108342361864</v>
+      </c>
+      <c r="DF13" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251113-tett6roof-probeadjusted</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>